<commit_message>
Ran individual models, performed data processing, updated data sanitizing to remove negative SF values
</commit_message>
<xml_diff>
--- a/data/modeling_data/cluster_statistics.xlsx
+++ b/data/modeling_data/cluster_statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\modeling_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4710AE01-FCB4-45AB-A70A-A19374D4275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A481D2FD-9E64-40EF-A994-DDC69B54DBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Woodland/Shrubland</t>
   </si>
@@ -43,46 +43,49 @@
     <t>Temperate grassland desert</t>
   </si>
   <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>VPD</t>
+  </si>
+  <si>
+    <t>PPFD</t>
+  </si>
+  <si>
     <t>SWC</t>
   </si>
   <si>
+    <t>Sap flux</t>
+  </si>
+  <si>
     <t>Mean</t>
   </si>
   <si>
     <t>Variance</t>
   </si>
   <si>
+    <t>K-Means 0</t>
+  </si>
+  <si>
+    <t>K-Means 1</t>
+  </si>
+  <si>
+    <t>K-Means 2</t>
+  </si>
+  <si>
+    <t>K-Means 3</t>
+  </si>
+  <si>
     <t>Deciduous</t>
   </si>
   <si>
     <t>Evergreen</t>
   </si>
   <si>
-    <t>K-Means 0</t>
-  </si>
-  <si>
-    <t>K-Means 1</t>
-  </si>
-  <si>
-    <t>K-Means 2</t>
-  </si>
-  <si>
-    <t>K-Means 3</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>VPD</t>
-  </si>
-  <si>
-    <t>PPFD</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Sap flux</t>
+    <t>Mixed</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -569,7 +572,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,14 +580,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,33 +941,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -974,703 +969,666 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
         <v>14.026697196711201</v>
       </c>
       <c r="C3" s="3">
         <v>0.80833812367924596</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>393.26234847946</v>
       </c>
       <c r="E3" s="3">
         <v>0.140528382182005</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>470.634716347081</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
         <v>25.679286796789299</v>
       </c>
       <c r="C4" s="3">
         <v>0.52797179872035604</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>359.54010333443301</v>
       </c>
       <c r="E4" s="3">
         <v>0.249210856671048</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>4262.67067891448</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
         <v>15.8431097294946</v>
       </c>
       <c r="C5" s="3">
         <v>0.479668849230381</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>264.54299726826798</v>
       </c>
       <c r="E5" s="3">
         <v>0.32893216866785302</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>2847.3308634431201</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3">
         <v>11.3194127268707</v>
       </c>
       <c r="C6" s="3">
         <v>0.45569312194720002</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>378.26232563087302</v>
       </c>
       <c r="E6" s="3">
         <v>0.20917951880888999</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>6886.2211250727796</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3">
+        <v>16.172008751596401</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.62402078269795203</v>
+      </c>
+      <c r="D7" s="3">
+        <v>399.98813058735902</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.23488847493172599</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1831.31521878731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <v>13.947902126940599</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.80810091987197497</v>
+      </c>
+      <c r="D8" s="3">
+        <v>376.21961893161199</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.16125788762926199</v>
+      </c>
+      <c r="F8" s="3">
+        <v>842.41710698567897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3">
+        <v>15.682883167459799</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.58909021952529095</v>
+      </c>
+      <c r="D9" s="3">
+        <v>356.99695206818399</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.159118294808859</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1273.03170285429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>13.706401510558299</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.60107584096614697</v>
+      </c>
+      <c r="D10" s="3">
+        <v>375.82126487020599</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.166036146302948</v>
+      </c>
+      <c r="F10" s="3">
+        <v>504.08816812222801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>13.037381870882999</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.50200626727762299</v>
+      </c>
+      <c r="D11" s="3">
+        <v>324.05421665032799</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.220966401606178</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1714.4770613656799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>25.679286796789299</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.52797179872035604</v>
+      </c>
+      <c r="D12" s="3">
+        <v>359.54010333443301</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.249210856671048</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4262.67067891448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <v>24.540174091042399</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.30433016133025</v>
+      </c>
+      <c r="D13" s="3">
+        <v>538.97126165309203</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.16049177512653101</v>
+      </c>
+      <c r="F13" s="3">
+        <v>398.47270869335699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>18.6862853992629</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.38224646230742</v>
+      </c>
+      <c r="D14" s="3">
+        <v>439.78727683885597</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.11053315215045301</v>
+      </c>
+      <c r="F14" s="3">
+        <v>917.32257692079099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7.5512610098195196</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.30618888768021002</v>
+      </c>
+      <c r="D15" s="3">
+        <v>369.089509498273</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.29980468441327401</v>
+      </c>
+      <c r="F15" s="3">
+        <v>789.21848486162799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <v>16.3672629162707</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.4066629818668199</v>
+      </c>
+      <c r="D16" s="3">
+        <v>451.16459825761501</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.6371479778875905E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>229.66737168810801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
-        <v>16.309334551227401</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.60157314029712605</v>
-      </c>
-      <c r="D7" s="4">
-        <v>399.94542005711997</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.206955906705627</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1690.8652249924301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4">
-        <v>14.0261485829151</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.78851441235692199</v>
-      </c>
-      <c r="D8" s="4">
-        <v>369.45137271206102</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.15959560040890999</v>
-      </c>
-      <c r="F8" s="4">
-        <v>856.92497692572999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3">
+        <v>75.630002658318404</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.73809197040599295</v>
+      </c>
+      <c r="D20" s="3">
+        <v>316966.71369647002</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8.0704559219090099E-3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>958349.78651220899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3">
+        <v>5.76573931244946</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.210043209647228</v>
+      </c>
+      <c r="D21" s="3">
+        <v>295199.75142757001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.3896783653406099E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>30243668.608750202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3">
+        <v>49.081829675766997</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.32480519802894797</v>
+      </c>
+      <c r="D22" s="3">
+        <v>181808.14815939101</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.7675032132845998E-2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>11843881.099816799</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3">
+        <v>39.813937591347198</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.422593088878155</v>
+      </c>
+      <c r="D23" s="3">
+        <v>354676.77163313603</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.3269853190848404E-3</v>
+      </c>
+      <c r="F23" s="3">
+        <v>69749152.471527502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3">
+        <v>67.650734577920204</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.45710580954170499</v>
+      </c>
+      <c r="D24" s="3">
+        <v>317113.96294398198</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.1979838797278399E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>10402432.822578499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3">
+        <v>72.657493608048398</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.76447852392706594</v>
+      </c>
+      <c r="D25" s="3">
+        <v>306451.46735371498</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.4259715485066E-2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5517647.8229641002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3">
+        <v>76.007501388179406</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.41517593642856798</v>
+      </c>
+      <c r="D26" s="3">
+        <v>269389.43210035202</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7.6989967951510904E-3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>7110122.2409191597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4">
-        <v>13.706401510558299</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.60107584096614697</v>
-      </c>
-      <c r="D9" s="4">
-        <v>375.82126487020599</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.166036146302948</v>
-      </c>
-      <c r="F9" s="4">
-        <v>504.08816812222801</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B27" s="3">
+        <v>53.676261111187102</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.44488305172997</v>
+      </c>
+      <c r="D27" s="3">
+        <v>300480.99271249899</v>
+      </c>
+      <c r="E27" s="3">
+        <v>6.7371794498415896E-3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1558611.88373842</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
-        <v>13.037381870882999</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.50200626727762299</v>
-      </c>
-      <c r="D10" s="4">
-        <v>324.05421665032799</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.220966401606178</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1714.4770613656799</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B28" s="3">
+        <v>81.983368310552606</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.31649200074701</v>
+      </c>
+      <c r="D28" s="3">
+        <v>252303.89151468701</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1.7283459515144699E-2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>11156973.3945348</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4">
-        <v>25.679286796789299</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.52797179872035604</v>
-      </c>
-      <c r="D11" s="4">
-        <v>359.54010333443301</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.249210856671048</v>
-      </c>
-      <c r="F11" s="4">
-        <v>4262.67067891448</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B29" s="3">
+        <v>5.76573931244946</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.210043209647228</v>
+      </c>
+      <c r="D29" s="3">
+        <v>295199.75142757001</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1.3896783653406099E-2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>30243668.608750202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="4">
-        <v>24.540174091042399</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.30433016133025</v>
-      </c>
-      <c r="D12" s="4">
-        <v>538.97126165309203</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.16049177512653101</v>
-      </c>
-      <c r="F12" s="4">
-        <v>398.47270869335699</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B30" s="3">
+        <v>36.159665358462199</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1.4825886850742001</v>
+      </c>
+      <c r="D30" s="3">
+        <v>412636.94370197703</v>
+      </c>
+      <c r="E30" s="3">
+        <v>6.2205450160834298E-3</v>
+      </c>
+      <c r="F30" s="3">
+        <v>440343.00763452402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="4">
-        <v>18.6862853992629</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1.38224646230742</v>
-      </c>
-      <c r="D13" s="4">
-        <v>439.78727683885597</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.11053315215045301</v>
-      </c>
-      <c r="F13" s="4">
-        <v>917.32257692079099</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B31" s="3">
+        <v>43.691616175915698</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1.2292251177864</v>
+      </c>
+      <c r="D31" s="3">
+        <v>364813.44047249999</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.6225627043731802E-3</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1585296.2045299499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4">
-        <v>7.5512610098195196</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.30618888768021002</v>
-      </c>
-      <c r="D14" s="4">
-        <v>369.089509498273</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.29980468441327401</v>
-      </c>
-      <c r="F14" s="4">
-        <v>789.21848486162799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B32" s="3">
+        <v>34.353748817391001</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.107692013857866</v>
+      </c>
+      <c r="D32" s="3">
+        <v>326422.54676938802</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1.3727527571620201E-2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1561931.1248296101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4">
-        <v>16.3672629162707</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.4066629818668199</v>
-      </c>
-      <c r="D15" s="4">
-        <v>451.16459825761501</v>
-      </c>
-      <c r="E15" s="3">
-        <v>6.6371479778875905E-2</v>
-      </c>
-      <c r="F15" s="4">
-        <v>229.66737168810801</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="3">
-        <v>8.6965511933362638</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.85912279122718715</v>
-      </c>
-      <c r="D19" s="4">
-        <v>562.99796953139185</v>
-      </c>
-      <c r="E19" s="3">
-        <v>8.9835716293181572E-2</v>
-      </c>
-      <c r="F19" s="4">
-        <v>978.95341386207394</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2.401195392393018</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.45830471266094136</v>
-      </c>
-      <c r="D20" s="4">
-        <v>543.32287953625701</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.11788462008848355</v>
-      </c>
-      <c r="F20" s="4">
-        <v>5499.424388856547</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3">
-        <v>7.0058425386078298</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.56991683430913664</v>
-      </c>
-      <c r="D21" s="4">
-        <v>426.38966704106588</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.1329474788510335</v>
-      </c>
-      <c r="F21" s="4">
-        <v>3441.4940214704425</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="3">
-        <v>6.3098286499196785</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.65007160288552446</v>
-      </c>
-      <c r="D22" s="4">
-        <v>595.54745539976579</v>
-      </c>
-      <c r="E22" s="3">
-        <v>6.5779824559547437E-2</v>
-      </c>
-      <c r="F22" s="4">
-        <v>8351.595803888471</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3">
-        <v>8.7347341261215785</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.63195270507931522</v>
-      </c>
-      <c r="D23" s="4">
-        <v>557.194925807103</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.11123344555284889</v>
-      </c>
-      <c r="F23" s="4">
-        <v>3222.8526464641382</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="3">
-        <v>8.4627364368732465</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.86261520557274496</v>
-      </c>
-      <c r="D24" s="4">
-        <v>546.87301189539608</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.11518489360004548</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2301.2134854000269</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="3">
-        <v>7.3264084728594749</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0.66699554101205949</v>
-      </c>
-      <c r="D25" s="4">
-        <v>548.1614659135563</v>
-      </c>
-      <c r="E25" s="3">
-        <v>8.2080323158730248E-2</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1248.4437847730348</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3">
-        <v>9.0544667601440008</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0.56257621772255006</v>
-      </c>
-      <c r="D26" s="4">
-        <v>502.29860791633399</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.13146657185438698</v>
-      </c>
-      <c r="F26" s="4">
-        <v>3340.2055916567174</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2.401195392393018</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0.45830471266094136</v>
-      </c>
-      <c r="D27" s="4">
-        <v>543.32287953625701</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0.11788462008848355</v>
-      </c>
-      <c r="F27" s="4">
-        <v>5499.424388856547</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3">
-        <v>6.0132907262548185</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1.2176159842389553</v>
-      </c>
-      <c r="D28" s="4">
-        <v>642.36823061385678</v>
-      </c>
-      <c r="E28" s="3">
-        <v>7.8870431823868131E-2</v>
-      </c>
-      <c r="F28" s="4">
-        <v>663.58345943409711</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3">
-        <v>6.6099634020103091</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1.1087042517219821</v>
-      </c>
-      <c r="D29" s="4">
-        <v>603.99788118212803</v>
-      </c>
-      <c r="E29" s="3">
-        <v>5.1210962736246035E-2</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1259.0854635527924</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="3">
-        <v>5.8612071126510283</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0.32816461396358076</v>
-      </c>
-      <c r="D30" s="4">
-        <v>571.33400631275924</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.11716453205479976</v>
-      </c>
-      <c r="F30" s="4">
-        <v>1249.7724292164594</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="3">
-        <v>8.1298111184474209</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1.0208756345578436</v>
-      </c>
-      <c r="D31" s="4">
-        <v>603.36460977583863</v>
-      </c>
-      <c r="E31" s="3">
-        <v>3.946552790543717E-2</v>
-      </c>
-      <c r="F31" s="4">
-        <v>308.45077564360946</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="6"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>66.093828821631305</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1.0421870612338799</v>
+      </c>
+      <c r="D33" s="3">
+        <v>364048.85232995002</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1.5575278928548399E-3</v>
+      </c>
+      <c r="F33" s="3">
+        <v>95141.880995144296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>